<commit_message>
user stories final edition
</commit_message>
<xml_diff>
--- a/Doc/User stories.xlsx
+++ b/Doc/User stories.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="88">
   <si>
     <t>ID</t>
   </si>
@@ -161,114 +161,9 @@
     <t>As a user, I want to get information about users</t>
   </si>
   <si>
-    <t xml:space="preserve">As a registred user, I want to add questions </t>
-  </si>
-  <si>
-    <t>As a registred user, I want to like answers</t>
-  </si>
-  <si>
-    <t>As a registred user, I want to cancel my likes</t>
-  </si>
-  <si>
-    <t>As a registered user, I want to attach vk.com account</t>
-  </si>
-  <si>
-    <t>As a registered user, I want to attach facebook.com account</t>
-  </si>
-  <si>
-    <t>As a registered user, I want to attach myspace.com account</t>
-  </si>
-  <si>
-    <t>As a registered user, I want to attach twitter.com account</t>
-  </si>
-  <si>
-    <t>As a registered user, I want to add a registerd user to my friendlist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a registered user, I want to  change background of my page </t>
-  </si>
-  <si>
-    <t>As a registered user, I want to  add my mude to my page</t>
-  </si>
-  <si>
-    <t>As a registered user, I want to change my personal information</t>
-  </si>
-  <si>
-    <t>As a registered user, I want to set privacy of my psage</t>
-  </si>
-  <si>
-    <t>As a registered user, I want to view incoming questions list</t>
-  </si>
-  <si>
-    <t>As a registered user, I want to choose incoming question, I want to answer</t>
-  </si>
-  <si>
-    <t>As a registered user, I want to write an answer on chosen question</t>
-  </si>
-  <si>
-    <t>As a registered user, I want to view number of my answers</t>
-  </si>
-  <si>
-    <t>As a registered user, I want to view number of my questions</t>
-  </si>
-  <si>
-    <t>As a registered user, I want to view number of my likes</t>
-  </si>
-  <si>
-    <t>As a registered user, I want to follow the page, I am interested in</t>
-  </si>
-  <si>
-    <t>As a registered user, I want to write a comment a chosen answer</t>
-  </si>
-  <si>
-    <t>As a user, I want to search registered users` pages by keywords</t>
-  </si>
-  <si>
-    <t>As a user, I want to filter the list of registered users` pages</t>
-  </si>
-  <si>
-    <t>As a registered user, I want to choose answer, I want to comment</t>
-  </si>
-  <si>
-    <t>As a user, I want to input my question on user`s page wall</t>
-  </si>
-  <si>
-    <t>As a user, I want to send my question</t>
-  </si>
-  <si>
-    <t>As a user, I want to report administrator about my problems</t>
-  </si>
-  <si>
-    <t>As an admin, I want to view the list of users` questions</t>
-  </si>
-  <si>
-    <t>As an admin, I want to choose user`s question</t>
-  </si>
-  <si>
-    <t>As an admin, I want to answer chosen user`s question</t>
-  </si>
-  <si>
     <t>As an admin, I want to  manage user list</t>
   </si>
   <si>
-    <t>As a registered user, I want to delete a registerd user to my friendlist</t>
-  </si>
-  <si>
-    <t>As an admin, I want to  deliver question of a day to all users</t>
-  </si>
-  <si>
-    <t>As an admin, I want to delete a registerd user to my friendlist</t>
-  </si>
-  <si>
-    <t>As an admin, I want to deliver system warnings</t>
-  </si>
-  <si>
-    <t>As an admin, I want to delete suspicious questions and answers</t>
-  </si>
-  <si>
-    <t>As an admin, I want to comment answers with administration warnings</t>
-  </si>
-  <si>
     <t xml:space="preserve">Implement, choose registered user </t>
   </si>
   <si>
@@ -327,6 +222,108 @@
   </si>
   <si>
     <t xml:space="preserve">AS OF 2014-10-03 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create textbox for add questions </t>
+  </si>
+  <si>
+    <t>Add "star"button to like answers</t>
+  </si>
+  <si>
+    <t>Double click "star"button to cancel my likes</t>
+  </si>
+  <si>
+    <t>Create icon-button to attach vk.com account</t>
+  </si>
+  <si>
+    <t>Create icon-button to attach facebook.com account</t>
+  </si>
+  <si>
+    <t>Create icon-button to attach myspace.com account</t>
+  </si>
+  <si>
+    <t>Create icon-button to attach twitter.com account</t>
+  </si>
+  <si>
+    <t>Create button in page to add a registerd user to my friendlist</t>
+  </si>
+  <si>
+    <t>Create "cross"button near friend to delete a registerd user to my friendlist</t>
+  </si>
+  <si>
+    <t>Change background of pages</t>
+  </si>
+  <si>
+    <t>Create special box, add mude to this box</t>
+  </si>
+  <si>
+    <t>In setting create a textbox's to change personal information</t>
+  </si>
+  <si>
+    <t>Realize privacity of page</t>
+  </si>
+  <si>
+    <t>Create incoming questions list</t>
+  </si>
+  <si>
+    <t>Realize textbox for answering the question</t>
+  </si>
+  <si>
+    <t>Realize amount of answer</t>
+  </si>
+  <si>
+    <t>Realize amount of  questions</t>
+  </si>
+  <si>
+    <t>Realize amount of  likes</t>
+  </si>
+  <si>
+    <t>Realize a follow pages</t>
+  </si>
+  <si>
+    <t>Realize comment to answers</t>
+  </si>
+  <si>
+    <t>Create special box for written a comment</t>
+  </si>
+  <si>
+    <t>Realize search by keyword in searchbox</t>
+  </si>
+  <si>
+    <t>Realize filtering</t>
+  </si>
+  <si>
+    <t>Create textbox for add questions to user in his page</t>
+  </si>
+  <si>
+    <t>Create button to send answer to user</t>
+  </si>
+  <si>
+    <t>Realize support system</t>
+  </si>
+  <si>
+    <t>Realize list of users' questions (support)</t>
+  </si>
+  <si>
+    <t>Realize choosen question to get information about it</t>
+  </si>
+  <si>
+    <t>Realize textbox to enter answer (support)</t>
+  </si>
+  <si>
+    <t>Realize delete a registerd user only for admin</t>
+  </si>
+  <si>
+    <t>Realize delivery question for all users</t>
+  </si>
+  <si>
+    <t>Realize sending a warning message</t>
+  </si>
+  <si>
+    <t>Realize delete suspicious questions and answers</t>
+  </si>
+  <si>
+    <t>Realize comment answers with administration status</t>
   </si>
 </sst>
 </file>
@@ -602,7 +599,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -904,17 +901,28 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color auto="1"/>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
-      <right style="thick">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
-      <bottom style="thick">
-        <color auto="1"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -925,7 +933,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -975,20 +983,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1000,30 +994,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -1040,21 +1013,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1066,17 +1030,8 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1085,21 +1040,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1108,9 +1054,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1118,9 +1061,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="19" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1130,92 +1070,151 @@
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Акцент1" xfId="1" builtinId="29"/>
@@ -1614,28 +1613,28 @@
   <sheetData>
     <row r="1" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
       <c r="E1" s="5"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="18"/>
+      <c r="C2" s="73"/>
       <c r="D2" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="19"/>
+      <c r="C3" s="74"/>
       <c r="D3" s="13" t="s">
         <v>4</v>
       </c>
@@ -1702,10 +1701,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BS60"/>
+  <dimension ref="A1:BS59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1717,36 +1716,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:71" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
     </row>
     <row r="2" spans="1:71" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" s="109" t="s">
-        <v>88</v>
+      <c r="B2" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="71" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:71" s="24" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" s="23" t="s">
+    <row r="4" spans="1:71" s="20" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="14"/>
@@ -1817,618 +1816,612 @@
       <c r="BS4" s="14"/>
     </row>
     <row r="5" spans="1:71" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25">
+      <c r="A5" s="21">
         <v>1</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="94" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="39"/>
+    </row>
+    <row r="6" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="22">
+        <v>2</v>
+      </c>
+      <c r="B6" s="97"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="37"/>
+    </row>
+    <row r="7" spans="1:71" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="22">
+        <v>3</v>
+      </c>
+      <c r="B7" s="97"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="37"/>
+    </row>
+    <row r="8" spans="1:71" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="22">
+        <v>4</v>
+      </c>
+      <c r="B8" s="97"/>
+      <c r="C8" s="98" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="35"/>
+    </row>
+    <row r="9" spans="1:71" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="22">
+        <v>5</v>
+      </c>
+      <c r="B9" s="97"/>
+      <c r="C9" s="98"/>
+      <c r="D9" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="35"/>
+    </row>
+    <row r="10" spans="1:71" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="22">
+        <v>6</v>
+      </c>
+      <c r="B10" s="97"/>
+      <c r="C10" s="98"/>
+      <c r="D10" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="35"/>
+    </row>
+    <row r="11" spans="1:71" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="22">
+        <v>7</v>
+      </c>
+      <c r="B11" s="97"/>
+      <c r="C11" s="98"/>
+      <c r="D11" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="35"/>
+    </row>
+    <row r="12" spans="1:71" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="22">
+        <v>8</v>
+      </c>
+      <c r="B12" s="97"/>
+      <c r="C12" s="99" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="36"/>
+    </row>
+    <row r="13" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22">
+        <v>9</v>
+      </c>
+      <c r="B13" s="97"/>
+      <c r="C13" s="99"/>
+      <c r="D13" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="36"/>
+    </row>
+    <row r="14" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="22">
+        <v>10</v>
+      </c>
+      <c r="B14" s="97"/>
+      <c r="C14" s="100" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="32"/>
+    </row>
+    <row r="15" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="68">
+        <v>11</v>
+      </c>
+      <c r="B15" s="97"/>
+      <c r="C15" s="101"/>
+      <c r="D15" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="32"/>
+    </row>
+    <row r="16" spans="1:71" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="69">
+        <v>12</v>
+      </c>
+      <c r="B16" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="102" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="41"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="70">
+        <v>13</v>
+      </c>
+      <c r="B17" s="93"/>
+      <c r="C17" s="91"/>
+      <c r="D17" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="41"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="70">
+        <v>14</v>
+      </c>
+      <c r="B18" s="93"/>
+      <c r="C18" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="45"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="70">
+        <v>15</v>
+      </c>
+      <c r="B19" s="93"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="45"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="70">
+        <v>16</v>
+      </c>
+      <c r="B20" s="93"/>
+      <c r="C20" s="89" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="47"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="70">
+        <v>17</v>
+      </c>
+      <c r="B21" s="93"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="47"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="70">
+        <v>18</v>
+      </c>
+      <c r="B22" s="93"/>
+      <c r="C22" s="90" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="50"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="70">
+        <v>19</v>
+      </c>
+      <c r="B23" s="93"/>
+      <c r="C23" s="90"/>
+      <c r="D23" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="50"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="70">
+        <v>20</v>
+      </c>
+      <c r="B24" s="93"/>
+      <c r="C24" s="90"/>
+      <c r="D24" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="50"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="70">
+        <v>21</v>
+      </c>
+      <c r="B25" s="93"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="50"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="70">
+        <v>22</v>
+      </c>
+      <c r="B26" s="93"/>
+      <c r="C26" s="91" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="41"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="70">
+        <v>23</v>
+      </c>
+      <c r="B27" s="93"/>
+      <c r="C27" s="91"/>
+      <c r="D27" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="41"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="70">
+        <v>24</v>
+      </c>
+      <c r="B28" s="93"/>
+      <c r="C28" s="92" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="45"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="70">
+        <v>25</v>
+      </c>
+      <c r="B29" s="93"/>
+      <c r="C29" s="92"/>
+      <c r="D29" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="45"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="70">
+        <v>26</v>
+      </c>
+      <c r="B30" s="93"/>
+      <c r="C30" s="92"/>
+      <c r="D30" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" s="45"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="70">
+        <v>27</v>
+      </c>
+      <c r="B31" s="93"/>
+      <c r="C31" s="92"/>
+      <c r="D31" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="45"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="70">
+        <v>28</v>
+      </c>
+      <c r="B32" s="93"/>
+      <c r="C32" s="92"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="45"/>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="70">
+        <v>29</v>
+      </c>
+      <c r="B33" s="93"/>
+      <c r="C33" s="105" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="47"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="70">
+        <v>30</v>
+      </c>
+      <c r="B34" s="93"/>
+      <c r="C34" s="106"/>
+      <c r="D34" s="103" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" s="104"/>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="70">
+        <v>31</v>
+      </c>
+      <c r="B35" s="93"/>
+      <c r="C35" s="90" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="54"/>
-    </row>
-    <row r="6" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27">
-        <v>2</v>
-      </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="35" t="s">
+      <c r="E35" s="50"/>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="70">
+        <v>32</v>
+      </c>
+      <c r="B36" s="93"/>
+      <c r="C36" s="90"/>
+      <c r="D36" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="51"/>
-    </row>
-    <row r="7" spans="1:71" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="27">
-        <v>3</v>
-      </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="35" t="s">
+      <c r="E36" s="50"/>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="70">
+        <v>33</v>
+      </c>
+      <c r="B37" s="93"/>
+      <c r="C37" s="90"/>
+      <c r="D37" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="51"/>
-    </row>
-    <row r="8" spans="1:71" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27">
-        <v>4</v>
-      </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="37" t="s">
+      <c r="E37" s="50"/>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="70">
+        <v>34</v>
+      </c>
+      <c r="B38" s="93"/>
+      <c r="C38" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="E8" s="49"/>
-    </row>
-    <row r="9" spans="1:71" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="27">
-        <v>5</v>
-      </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="37" t="s">
+      <c r="E38" s="41"/>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="70">
+        <v>35</v>
+      </c>
+      <c r="B39" s="93"/>
+      <c r="C39" s="81" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="49"/>
-    </row>
-    <row r="10" spans="1:71" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27">
-        <v>6</v>
-      </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="37" t="s">
+      <c r="E39" s="45"/>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="70">
+        <v>36</v>
+      </c>
+      <c r="B40" s="93"/>
+      <c r="C40" s="82"/>
+      <c r="D40" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="49"/>
-    </row>
-    <row r="11" spans="1:71" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="27">
-        <v>7</v>
-      </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="37" t="s">
+      <c r="E40" s="45"/>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="70">
+        <v>37</v>
+      </c>
+      <c r="B41" s="75" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="79" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="57" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="49"/>
-    </row>
-    <row r="12" spans="1:71" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27">
-        <v>8</v>
-      </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="40" t="s">
+      <c r="E41" s="58"/>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="70">
+        <v>38</v>
+      </c>
+      <c r="B42" s="75"/>
+      <c r="C42" s="80"/>
+      <c r="D42" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="50"/>
-    </row>
-    <row r="13" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="27">
-        <v>9</v>
-      </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="41" t="s">
+      <c r="E42" s="58"/>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="70">
+        <v>39</v>
+      </c>
+      <c r="B43" s="75"/>
+      <c r="C43" s="83" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="E13" s="50"/>
-    </row>
-    <row r="14" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27">
+      <c r="E43" s="61"/>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="70">
+        <v>40</v>
+      </c>
+      <c r="B44" s="75"/>
+      <c r="C44" s="83"/>
+      <c r="D44" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="E44" s="61"/>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="70">
+        <v>41</v>
+      </c>
+      <c r="B45" s="75"/>
+      <c r="C45" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="E45" s="33"/>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="70">
+        <v>42</v>
+      </c>
+      <c r="B46" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="43" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" s="46"/>
-    </row>
-    <row r="15" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="105">
+      <c r="C46" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" s="46"/>
-    </row>
-    <row r="16" spans="1:71" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="106">
+      <c r="D46" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="E46" s="34"/>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="70">
+        <v>43</v>
+      </c>
+      <c r="B47" s="76"/>
+      <c r="C47" s="85"/>
+      <c r="D47" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="E47" s="34"/>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="70">
+        <v>44</v>
+      </c>
+      <c r="B48" s="76"/>
+      <c r="C48" s="85"/>
+      <c r="D48" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E48" s="34"/>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="70">
+        <v>45</v>
+      </c>
+      <c r="B49" s="76"/>
+      <c r="C49" s="64" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E49" s="62"/>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="70">
+        <v>46</v>
+      </c>
+      <c r="B50" s="76"/>
+      <c r="C50" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="56" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="57" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="58"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="107">
+      <c r="D50" s="65" t="s">
+        <v>84</v>
+      </c>
+      <c r="E50" s="66"/>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="70">
+        <v>47</v>
+      </c>
+      <c r="B51" s="76"/>
+      <c r="C51" s="86"/>
+      <c r="D51" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="E51" s="66"/>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="70">
+        <v>48</v>
+      </c>
+      <c r="B52" s="76"/>
+      <c r="C52" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="55"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="60" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="58"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="107">
-        <v>14</v>
-      </c>
-      <c r="B18" s="55"/>
-      <c r="C18" s="62" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="63" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" s="64"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="107">
-        <v>15</v>
-      </c>
-      <c r="B19" s="55"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="63" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="64"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="107">
-        <v>16</v>
-      </c>
-      <c r="B20" s="55"/>
-      <c r="C20" s="65" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="66" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="67"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="107">
-        <v>17</v>
-      </c>
-      <c r="B21" s="55"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="66" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="67"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="107">
-        <v>18</v>
-      </c>
-      <c r="B22" s="55"/>
-      <c r="C22" s="69" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="70" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="71"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="107">
-        <v>19</v>
-      </c>
-      <c r="B23" s="55"/>
-      <c r="C23" s="69"/>
-      <c r="D23" s="70" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="71"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="107">
-        <v>20</v>
-      </c>
-      <c r="B24" s="55"/>
-      <c r="C24" s="69"/>
-      <c r="D24" s="70" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="71"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="107">
-        <v>21</v>
-      </c>
-      <c r="B25" s="55"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="70" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="71"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="107">
-        <v>22</v>
-      </c>
-      <c r="B26" s="55"/>
-      <c r="C26" s="59" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="61" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" s="58"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="107">
-        <v>23</v>
-      </c>
-      <c r="B27" s="55"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="E27" s="58"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="107">
-        <v>24</v>
-      </c>
-      <c r="B28" s="55"/>
-      <c r="C28" s="73" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="74" t="s">
-        <v>41</v>
-      </c>
-      <c r="E28" s="64"/>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="107">
-        <v>25</v>
-      </c>
-      <c r="B29" s="55"/>
-      <c r="C29" s="73"/>
-      <c r="D29" s="74" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29" s="64"/>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="107">
-        <v>26</v>
-      </c>
-      <c r="B30" s="55"/>
-      <c r="C30" s="73"/>
-      <c r="D30" s="74" t="s">
-        <v>43</v>
-      </c>
-      <c r="E30" s="64"/>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="107">
-        <v>27</v>
-      </c>
-      <c r="B31" s="55"/>
-      <c r="C31" s="73"/>
-      <c r="D31" s="74" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" s="64"/>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="107">
-        <v>28</v>
-      </c>
-      <c r="B32" s="55"/>
-      <c r="C32" s="73"/>
-      <c r="D32" s="74"/>
-      <c r="E32" s="64"/>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="107">
-        <v>29</v>
-      </c>
-      <c r="B33" s="55"/>
-      <c r="C33" s="65" t="s">
-        <v>19</v>
-      </c>
-      <c r="D33" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="E33" s="67"/>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="107">
-        <v>30</v>
-      </c>
-      <c r="B34" s="55"/>
-      <c r="C34" s="65"/>
-      <c r="D34" s="68" t="s">
-        <v>46</v>
-      </c>
-      <c r="E34" s="67"/>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="107">
-        <v>31</v>
-      </c>
-      <c r="B35" s="55"/>
-      <c r="C35" s="65"/>
-      <c r="D35" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="E35" s="67"/>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="107">
-        <v>32</v>
-      </c>
-      <c r="B36" s="55"/>
-      <c r="C36" s="69" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="70" t="s">
-        <v>48</v>
-      </c>
-      <c r="E36" s="71"/>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="107">
-        <v>33</v>
-      </c>
-      <c r="B37" s="55"/>
-      <c r="C37" s="69"/>
-      <c r="D37" s="70" t="s">
+      <c r="D52" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" s="38"/>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="70">
         <v>49</v>
       </c>
-      <c r="E37" s="71"/>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="107">
-        <v>34</v>
-      </c>
-      <c r="B38" s="55"/>
-      <c r="C38" s="69"/>
-      <c r="D38" s="70" t="s">
-        <v>50</v>
-      </c>
-      <c r="E38" s="71"/>
-    </row>
-    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="107">
-        <v>35</v>
-      </c>
-      <c r="B39" s="55"/>
-      <c r="C39" s="60" t="s">
-        <v>25</v>
-      </c>
-      <c r="D39" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="E39" s="58"/>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="107">
-        <v>36</v>
-      </c>
-      <c r="B40" s="55"/>
-      <c r="C40" s="62" t="s">
-        <v>26</v>
-      </c>
-      <c r="D40" s="75" t="s">
-        <v>55</v>
-      </c>
-      <c r="E40" s="64"/>
-    </row>
-    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="108">
-        <v>37</v>
-      </c>
-      <c r="B41" s="55"/>
-      <c r="C41" s="77"/>
-      <c r="D41" s="78" t="s">
-        <v>52</v>
-      </c>
-      <c r="E41" s="64"/>
-    </row>
-    <row r="42" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="102">
-        <v>38</v>
-      </c>
-      <c r="B42" s="80" t="s">
-        <v>32</v>
-      </c>
-      <c r="C42" s="81" t="s">
-        <v>21</v>
-      </c>
-      <c r="D42" s="82" t="s">
-        <v>53</v>
-      </c>
-      <c r="E42" s="83"/>
-    </row>
-    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="103">
-        <v>39</v>
-      </c>
-      <c r="B43" s="80"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="84" t="s">
-        <v>54</v>
-      </c>
-      <c r="E43" s="83"/>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="103">
-        <v>40</v>
-      </c>
-      <c r="B44" s="80"/>
-      <c r="C44" s="85" t="s">
-        <v>22</v>
-      </c>
-      <c r="D44" s="86" t="s">
-        <v>56</v>
-      </c>
-      <c r="E44" s="87"/>
-    </row>
-    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="103">
-        <v>41</v>
-      </c>
-      <c r="B45" s="80"/>
-      <c r="C45" s="85"/>
-      <c r="D45" s="86" t="s">
-        <v>57</v>
-      </c>
-      <c r="E45" s="87"/>
-    </row>
-    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="104">
-        <v>42</v>
-      </c>
-      <c r="B46" s="80"/>
-      <c r="C46" s="79" t="s">
-        <v>23</v>
-      </c>
-      <c r="D46" s="79" t="s">
-        <v>58</v>
-      </c>
-      <c r="E46" s="47"/>
-    </row>
-    <row r="47" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="99">
-        <v>43</v>
-      </c>
-      <c r="B47" s="89" t="s">
-        <v>10</v>
-      </c>
-      <c r="C47" s="91" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" s="92" t="s">
-        <v>59</v>
-      </c>
-      <c r="E47" s="48"/>
-    </row>
-    <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="100">
-        <v>44</v>
-      </c>
-      <c r="B48" s="89"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="E48" s="48"/>
-    </row>
-    <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="100">
-        <v>45</v>
-      </c>
-      <c r="B49" s="89"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="E49" s="48"/>
-    </row>
-    <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="100">
-        <v>46</v>
-      </c>
-      <c r="B50" s="89"/>
-      <c r="C50" s="93" t="s">
-        <v>62</v>
-      </c>
-      <c r="D50" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="E50" s="88"/>
-    </row>
-    <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="100">
-        <v>47</v>
-      </c>
-      <c r="B51" s="89"/>
-      <c r="C51" s="94" t="s">
-        <v>12</v>
-      </c>
-      <c r="D51" s="95" t="s">
-        <v>64</v>
-      </c>
-      <c r="E51" s="96"/>
-    </row>
-    <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="100">
-        <v>48</v>
-      </c>
-      <c r="B52" s="89"/>
-      <c r="C52" s="94"/>
-      <c r="D52" s="95" t="s">
-        <v>66</v>
-      </c>
-      <c r="E52" s="96"/>
-    </row>
-    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="100">
-        <v>49</v>
-      </c>
-      <c r="B53" s="89"/>
-      <c r="C53" s="52" t="s">
-        <v>13</v>
-      </c>
-      <c r="D53" s="72" t="s">
-        <v>67</v>
-      </c>
-      <c r="E53" s="53"/>
-    </row>
-    <row r="54" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="101">
-        <v>50</v>
-      </c>
-      <c r="B54" s="90"/>
-      <c r="C54" s="97"/>
-      <c r="D54" s="76" t="s">
-        <v>68</v>
-      </c>
-      <c r="E54" s="98"/>
-    </row>
-    <row r="55" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="77"/>
+      <c r="C53" s="88"/>
+      <c r="D53" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="E53" s="67"/>
+    </row>
+    <row r="54" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="15"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="16"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B55" s="15"/>
       <c r="C55" s="14"/>
-      <c r="D55" s="16"/>
+      <c r="D55" s="14"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B56" s="15"/>
       <c r="C56" s="14"/>
       <c r="D56" s="14"/>
+      <c r="E56" s="16"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B57" s="15"/>
       <c r="C57" s="14"/>
       <c r="D57" s="14"/>
-      <c r="E57" s="16"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B58" s="15"/>
@@ -2436,38 +2429,33 @@
       <c r="D58" s="14"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B59" s="15"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F60" s="15"/>
+      <c r="F59" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B42:B46"/>
-    <mergeCell ref="B47:B54"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C32"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="B16:B41"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C33:C34"/>
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="B5:B15"/>
     <mergeCell ref="C8:C11"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="B46:B53"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C32"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="B16:B40"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
final backlog and changed user-stories
backlog is almost ready(change russian text for english), user stories-
ready
</commit_message>
<xml_diff>
--- a/Doc/User stories.xlsx
+++ b/Doc/User stories.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Дмитрий\Documents\GitHub\Ask_service\Doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9570" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20730" windowHeight="9510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +26,7 @@
     <author>Henrik</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -245,21 +240,12 @@
     <t>Create icon-button to attach twitter.com account</t>
   </si>
   <si>
-    <t>Create button in page to add a registerd user to my friendlist</t>
-  </si>
-  <si>
-    <t>Create "cross"button near friend to delete a registerd user to my friendlist</t>
-  </si>
-  <si>
     <t>Change background of pages</t>
   </si>
   <si>
     <t>Create special box, add mude to this box</t>
   </si>
   <si>
-    <t>In setting create a textbox's to change personal information</t>
-  </si>
-  <si>
     <t>Realize privacity of page</t>
   </si>
   <si>
@@ -311,9 +297,6 @@
     <t>Realize textbox to enter answer (support)</t>
   </si>
   <si>
-    <t>Realize delete a registerd user only for admin</t>
-  </si>
-  <si>
     <t>Realize delivery question for all users</t>
   </si>
   <si>
@@ -324,6 +307,18 @@
   </si>
   <si>
     <t>Realize comment answers with administration status</t>
+  </si>
+  <si>
+    <t>Create button in page to add a registred user to my friendlist</t>
+  </si>
+  <si>
+    <t>Create "cross"button near friend to delete a registred user to my friendlist</t>
+  </si>
+  <si>
+    <t>In settings create a textbox's to change personal information</t>
+  </si>
+  <si>
+    <t>Realize delete a registred user only for admin</t>
   </si>
 </sst>
 </file>
@@ -1108,6 +1103,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1119,6 +1120,45 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1137,9 +1177,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1167,52 +1204,10 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="19" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1351,7 +1346,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1386,7 +1381,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1613,28 +1608,28 @@
   <sheetData>
     <row r="1" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
       <c r="E1" s="5"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="73"/>
+      <c r="C2" s="75"/>
       <c r="D2" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="74"/>
+      <c r="C3" s="76"/>
       <c r="D3" s="13" t="s">
         <v>4</v>
       </c>
@@ -1703,8 +1698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BS59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="C38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1716,12 +1711,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:71" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
     </row>
     <row r="2" spans="1:71" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B2" s="17" t="s">
@@ -1819,10 +1814,10 @@
       <c r="A5" s="21">
         <v>1</v>
       </c>
-      <c r="B5" s="96" t="s">
+      <c r="B5" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="94" t="s">
+      <c r="C5" s="82" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="23" t="s">
@@ -1834,8 +1829,8 @@
       <c r="A6" s="22">
         <v>2</v>
       </c>
-      <c r="B6" s="97"/>
-      <c r="C6" s="95"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="83"/>
       <c r="D6" s="24" t="s">
         <v>35</v>
       </c>
@@ -1845,8 +1840,8 @@
       <c r="A7" s="22">
         <v>3</v>
       </c>
-      <c r="B7" s="97"/>
-      <c r="C7" s="95"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="83"/>
       <c r="D7" s="24" t="s">
         <v>36</v>
       </c>
@@ -1856,8 +1851,8 @@
       <c r="A8" s="22">
         <v>4</v>
       </c>
-      <c r="B8" s="97"/>
-      <c r="C8" s="98" t="s">
+      <c r="B8" s="85"/>
+      <c r="C8" s="86" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="26" t="s">
@@ -1869,8 +1864,8 @@
       <c r="A9" s="22">
         <v>5</v>
       </c>
-      <c r="B9" s="97"/>
-      <c r="C9" s="98"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="86"/>
       <c r="D9" s="26" t="s">
         <v>38</v>
       </c>
@@ -1880,8 +1875,8 @@
       <c r="A10" s="22">
         <v>6</v>
       </c>
-      <c r="B10" s="97"/>
-      <c r="C10" s="98"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="86"/>
       <c r="D10" s="26" t="s">
         <v>39</v>
       </c>
@@ -1891,8 +1886,8 @@
       <c r="A11" s="22">
         <v>7</v>
       </c>
-      <c r="B11" s="97"/>
-      <c r="C11" s="98"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="86"/>
       <c r="D11" s="26" t="s">
         <v>40</v>
       </c>
@@ -1902,8 +1897,8 @@
       <c r="A12" s="22">
         <v>8</v>
       </c>
-      <c r="B12" s="97"/>
-      <c r="C12" s="99" t="s">
+      <c r="B12" s="85"/>
+      <c r="C12" s="87" t="s">
         <v>29</v>
       </c>
       <c r="D12" s="28" t="s">
@@ -1915,8 +1910,8 @@
       <c r="A13" s="22">
         <v>9</v>
       </c>
-      <c r="B13" s="97"/>
-      <c r="C13" s="99"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="87"/>
       <c r="D13" s="29" t="s">
         <v>42</v>
       </c>
@@ -1926,8 +1921,8 @@
       <c r="A14" s="22">
         <v>10</v>
       </c>
-      <c r="B14" s="97"/>
-      <c r="C14" s="100" t="s">
+      <c r="B14" s="85"/>
+      <c r="C14" s="88" t="s">
         <v>30</v>
       </c>
       <c r="D14" s="30" t="s">
@@ -1939,8 +1934,8 @@
       <c r="A15" s="68">
         <v>11</v>
       </c>
-      <c r="B15" s="97"/>
-      <c r="C15" s="101"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="89"/>
       <c r="D15" s="31" t="s">
         <v>44</v>
       </c>
@@ -1950,10 +1945,10 @@
       <c r="A16" s="69">
         <v>12</v>
       </c>
-      <c r="B16" s="93" t="s">
+      <c r="B16" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="102" t="s">
+      <c r="C16" s="77" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="40" t="s">
@@ -1965,8 +1960,8 @@
       <c r="A17" s="70">
         <v>13</v>
       </c>
-      <c r="B17" s="93"/>
-      <c r="C17" s="91"/>
+      <c r="B17" s="106"/>
+      <c r="C17" s="78"/>
       <c r="D17" s="42" t="s">
         <v>46</v>
       </c>
@@ -1976,8 +1971,8 @@
       <c r="A18" s="70">
         <v>14</v>
       </c>
-      <c r="B18" s="93"/>
-      <c r="C18" s="81" t="s">
+      <c r="B18" s="106"/>
+      <c r="C18" s="79" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="44" t="s">
@@ -1989,8 +1984,8 @@
       <c r="A19" s="70">
         <v>15</v>
       </c>
-      <c r="B19" s="93"/>
-      <c r="C19" s="81"/>
+      <c r="B19" s="106"/>
+      <c r="C19" s="79"/>
       <c r="D19" s="44" t="s">
         <v>54</v>
       </c>
@@ -2000,8 +1995,8 @@
       <c r="A20" s="70">
         <v>16</v>
       </c>
-      <c r="B20" s="93"/>
-      <c r="C20" s="89" t="s">
+      <c r="B20" s="106"/>
+      <c r="C20" s="103" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="46" t="s">
@@ -2013,8 +2008,8 @@
       <c r="A21" s="70">
         <v>17</v>
       </c>
-      <c r="B21" s="93"/>
-      <c r="C21" s="89"/>
+      <c r="B21" s="106"/>
+      <c r="C21" s="103"/>
       <c r="D21" s="46" t="s">
         <v>56</v>
       </c>
@@ -2024,8 +2019,8 @@
       <c r="A22" s="70">
         <v>18</v>
       </c>
-      <c r="B22" s="93"/>
-      <c r="C22" s="90" t="s">
+      <c r="B22" s="106"/>
+      <c r="C22" s="104" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="49" t="s">
@@ -2037,8 +2032,8 @@
       <c r="A23" s="70">
         <v>19</v>
       </c>
-      <c r="B23" s="93"/>
-      <c r="C23" s="90"/>
+      <c r="B23" s="106"/>
+      <c r="C23" s="104"/>
       <c r="D23" s="49" t="s">
         <v>58</v>
       </c>
@@ -2048,8 +2043,8 @@
       <c r="A24" s="70">
         <v>20</v>
       </c>
-      <c r="B24" s="93"/>
-      <c r="C24" s="90"/>
+      <c r="B24" s="106"/>
+      <c r="C24" s="104"/>
       <c r="D24" s="49" t="s">
         <v>59</v>
       </c>
@@ -2059,8 +2054,8 @@
       <c r="A25" s="70">
         <v>21</v>
       </c>
-      <c r="B25" s="93"/>
-      <c r="C25" s="90"/>
+      <c r="B25" s="106"/>
+      <c r="C25" s="104"/>
       <c r="D25" s="49" t="s">
         <v>60</v>
       </c>
@@ -2070,12 +2065,12 @@
       <c r="A26" s="70">
         <v>22</v>
       </c>
-      <c r="B26" s="93"/>
-      <c r="C26" s="91" t="s">
+      <c r="B26" s="106"/>
+      <c r="C26" s="78" t="s">
         <v>17</v>
       </c>
       <c r="D26" s="43" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="E26" s="41"/>
     </row>
@@ -2083,10 +2078,10 @@
       <c r="A27" s="70">
         <v>23</v>
       </c>
-      <c r="B27" s="93"/>
-      <c r="C27" s="91"/>
+      <c r="B27" s="106"/>
+      <c r="C27" s="78"/>
       <c r="D27" s="43" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="E27" s="41"/>
     </row>
@@ -2094,12 +2089,12 @@
       <c r="A28" s="70">
         <v>24</v>
       </c>
-      <c r="B28" s="93"/>
-      <c r="C28" s="92" t="s">
+      <c r="B28" s="106"/>
+      <c r="C28" s="105" t="s">
         <v>18</v>
       </c>
       <c r="D28" s="52" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E28" s="45"/>
     </row>
@@ -2107,10 +2102,10 @@
       <c r="A29" s="70">
         <v>25</v>
       </c>
-      <c r="B29" s="93"/>
-      <c r="C29" s="92"/>
+      <c r="B29" s="106"/>
+      <c r="C29" s="105"/>
       <c r="D29" s="52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E29" s="45"/>
     </row>
@@ -2118,10 +2113,10 @@
       <c r="A30" s="70">
         <v>26</v>
       </c>
-      <c r="B30" s="93"/>
-      <c r="C30" s="92"/>
+      <c r="B30" s="106"/>
+      <c r="C30" s="105"/>
       <c r="D30" s="52" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="E30" s="45"/>
     </row>
@@ -2129,10 +2124,10 @@
       <c r="A31" s="70">
         <v>27</v>
       </c>
-      <c r="B31" s="93"/>
-      <c r="C31" s="92"/>
+      <c r="B31" s="106"/>
+      <c r="C31" s="105"/>
       <c r="D31" s="52" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E31" s="45"/>
     </row>
@@ -2140,8 +2135,8 @@
       <c r="A32" s="70">
         <v>28</v>
       </c>
-      <c r="B32" s="93"/>
-      <c r="C32" s="92"/>
+      <c r="B32" s="106"/>
+      <c r="C32" s="105"/>
       <c r="D32" s="52"/>
       <c r="E32" s="45"/>
     </row>
@@ -2149,12 +2144,12 @@
       <c r="A33" s="70">
         <v>29</v>
       </c>
-      <c r="B33" s="93"/>
-      <c r="C33" s="105" t="s">
+      <c r="B33" s="106"/>
+      <c r="C33" s="80" t="s">
         <v>19</v>
       </c>
       <c r="D33" s="48" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E33" s="47"/>
     </row>
@@ -2162,23 +2157,23 @@
       <c r="A34" s="70">
         <v>30</v>
       </c>
-      <c r="B34" s="93"/>
-      <c r="C34" s="106"/>
-      <c r="D34" s="103" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" s="104"/>
+      <c r="B34" s="106"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="72" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="73"/>
     </row>
     <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="70">
         <v>31</v>
       </c>
-      <c r="B35" s="93"/>
-      <c r="C35" s="90" t="s">
+      <c r="B35" s="106"/>
+      <c r="C35" s="104" t="s">
         <v>24</v>
       </c>
       <c r="D35" s="49" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E35" s="50"/>
     </row>
@@ -2186,10 +2181,10 @@
       <c r="A36" s="70">
         <v>32</v>
       </c>
-      <c r="B36" s="93"/>
-      <c r="C36" s="90"/>
+      <c r="B36" s="106"/>
+      <c r="C36" s="104"/>
       <c r="D36" s="49" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E36" s="50"/>
     </row>
@@ -2197,10 +2192,10 @@
       <c r="A37" s="70">
         <v>33</v>
       </c>
-      <c r="B37" s="93"/>
-      <c r="C37" s="90"/>
+      <c r="B37" s="106"/>
+      <c r="C37" s="104"/>
       <c r="D37" s="49" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E37" s="50"/>
     </row>
@@ -2208,12 +2203,12 @@
       <c r="A38" s="70">
         <v>34</v>
       </c>
-      <c r="B38" s="93"/>
+      <c r="B38" s="106"/>
       <c r="C38" s="42" t="s">
         <v>25</v>
       </c>
       <c r="D38" s="43" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E38" s="41"/>
     </row>
@@ -2221,12 +2216,12 @@
       <c r="A39" s="70">
         <v>35</v>
       </c>
-      <c r="B39" s="93"/>
-      <c r="C39" s="81" t="s">
+      <c r="B39" s="106"/>
+      <c r="C39" s="79" t="s">
         <v>26</v>
       </c>
       <c r="D39" s="53" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E39" s="45"/>
     </row>
@@ -2234,10 +2229,10 @@
       <c r="A40" s="70">
         <v>36</v>
       </c>
-      <c r="B40" s="93"/>
-      <c r="C40" s="82"/>
+      <c r="B40" s="106"/>
+      <c r="C40" s="96"/>
       <c r="D40" s="55" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E40" s="45"/>
     </row>
@@ -2245,14 +2240,14 @@
       <c r="A41" s="70">
         <v>37</v>
       </c>
-      <c r="B41" s="75" t="s">
+      <c r="B41" s="90" t="s">
         <v>32</v>
       </c>
-      <c r="C41" s="79" t="s">
+      <c r="C41" s="94" t="s">
         <v>21</v>
       </c>
       <c r="D41" s="57" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E41" s="58"/>
     </row>
@@ -2260,10 +2255,10 @@
       <c r="A42" s="70">
         <v>38</v>
       </c>
-      <c r="B42" s="75"/>
-      <c r="C42" s="80"/>
+      <c r="B42" s="90"/>
+      <c r="C42" s="95"/>
       <c r="D42" s="59" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E42" s="58"/>
     </row>
@@ -2271,12 +2266,12 @@
       <c r="A43" s="70">
         <v>39</v>
       </c>
-      <c r="B43" s="75"/>
-      <c r="C43" s="83" t="s">
+      <c r="B43" s="90"/>
+      <c r="C43" s="97" t="s">
         <v>22</v>
       </c>
       <c r="D43" s="60" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E43" s="61"/>
     </row>
@@ -2284,10 +2279,10 @@
       <c r="A44" s="70">
         <v>40</v>
       </c>
-      <c r="B44" s="75"/>
-      <c r="C44" s="83"/>
+      <c r="B44" s="90"/>
+      <c r="C44" s="97"/>
       <c r="D44" s="60" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E44" s="61"/>
     </row>
@@ -2295,12 +2290,12 @@
       <c r="A45" s="70">
         <v>41</v>
       </c>
-      <c r="B45" s="75"/>
+      <c r="B45" s="90"/>
       <c r="C45" s="56" t="s">
         <v>23</v>
       </c>
       <c r="D45" s="56" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E45" s="33"/>
     </row>
@@ -2308,14 +2303,14 @@
       <c r="A46" s="70">
         <v>42</v>
       </c>
-      <c r="B46" s="76" t="s">
+      <c r="B46" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="C46" s="84" t="s">
+      <c r="C46" s="98" t="s">
         <v>11</v>
       </c>
       <c r="D46" s="63" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E46" s="34"/>
     </row>
@@ -2323,10 +2318,10 @@
       <c r="A47" s="70">
         <v>43</v>
       </c>
-      <c r="B47" s="76"/>
-      <c r="C47" s="85"/>
+      <c r="B47" s="91"/>
+      <c r="C47" s="99"/>
       <c r="D47" s="27" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E47" s="34"/>
     </row>
@@ -2334,10 +2329,10 @@
       <c r="A48" s="70">
         <v>44</v>
       </c>
-      <c r="B48" s="76"/>
-      <c r="C48" s="85"/>
+      <c r="B48" s="91"/>
+      <c r="C48" s="99"/>
       <c r="D48" s="27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E48" s="34"/>
     </row>
@@ -2345,12 +2340,12 @@
       <c r="A49" s="70">
         <v>45</v>
       </c>
-      <c r="B49" s="76"/>
+      <c r="B49" s="91"/>
       <c r="C49" s="64" t="s">
         <v>33</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E49" s="62"/>
     </row>
@@ -2358,12 +2353,12 @@
       <c r="A50" s="70">
         <v>46</v>
       </c>
-      <c r="B50" s="76"/>
-      <c r="C50" s="86" t="s">
+      <c r="B50" s="91"/>
+      <c r="C50" s="100" t="s">
         <v>12</v>
       </c>
       <c r="D50" s="65" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E50" s="66"/>
     </row>
@@ -2371,10 +2366,10 @@
       <c r="A51" s="70">
         <v>47</v>
       </c>
-      <c r="B51" s="76"/>
-      <c r="C51" s="86"/>
+      <c r="B51" s="91"/>
+      <c r="C51" s="100"/>
       <c r="D51" s="65" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E51" s="66"/>
     </row>
@@ -2382,12 +2377,12 @@
       <c r="A52" s="70">
         <v>48</v>
       </c>
-      <c r="B52" s="76"/>
-      <c r="C52" s="87" t="s">
+      <c r="B52" s="91"/>
+      <c r="C52" s="101" t="s">
         <v>13</v>
       </c>
       <c r="D52" s="51" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E52" s="38"/>
     </row>
@@ -2395,10 +2390,10 @@
       <c r="A53" s="70">
         <v>49</v>
       </c>
-      <c r="B53" s="77"/>
-      <c r="C53" s="88"/>
+      <c r="B53" s="92"/>
+      <c r="C53" s="102"/>
       <c r="D53" s="54" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E53" s="67"/>
     </row>
@@ -2433,14 +2428,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B5:B15"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C14:C15"/>
     <mergeCell ref="B41:B45"/>
     <mergeCell ref="B46:B53"/>
     <mergeCell ref="B1:E1"/>
@@ -2456,6 +2443,14 @@
     <mergeCell ref="C28:C32"/>
     <mergeCell ref="C35:C37"/>
     <mergeCell ref="B16:B40"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B5:B15"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C15"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>